<commit_message>
updates to manuscript revision including analysis of carbon use in buried reaches 23-Jun-17
</commit_message>
<xml_diff>
--- a/cincy.reach.xlsx
+++ b/cincy.reach.xlsx
@@ -5,19 +5,20 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ArangoC\Dropbox\Cincinnati-R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ArangoC\Documents\R Files\Cinn R dev\Cincy-Carbon-Limitation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2235" windowWidth="26325" windowHeight="13620" activeTab="2"/>
+    <workbookView xWindow="2205" yWindow="2235" windowWidth="26325" windowHeight="13620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
     <sheet name="summary" sheetId="1" r:id="rId2"/>
     <sheet name="combined" sheetId="2" r:id="rId3"/>
+    <sheet name="bacterial growth efficiency" sheetId="4" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -546,7 +547,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="162">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1042,6 +1043,33 @@
   <si>
     <t>control.cr.afdm</t>
   </si>
+  <si>
+    <t>DOC (mg/L)</t>
+  </si>
+  <si>
+    <t>Q (L/s)</t>
+  </si>
+  <si>
+    <t>DOC (mg/s)</t>
+  </si>
+  <si>
+    <t>Whole-stream Respiration (g O2 m-2 d-1)</t>
+  </si>
+  <si>
+    <t>Whole-stream Respiration (g C m-2 d-1)</t>
+  </si>
+  <si>
+    <t>w (m)</t>
+  </si>
+  <si>
+    <t>Whole-stream Respiration (mg C m-2 s-1)</t>
+  </si>
+  <si>
+    <t>sw.m</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
 </sst>
 </file>
 
@@ -46227,11 +46255,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DS41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
+      <selection pane="bottomRight" activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52474,4 +52502,914 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" t="s">
+        <v>159</v>
+      </c>
+      <c r="K1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>combined!B2</f>
+        <v>Amberly</v>
+      </c>
+      <c r="B2" t="str">
+        <f>combined!C2</f>
+        <v>Fall</v>
+      </c>
+      <c r="C2" t="str">
+        <f>combined!D2</f>
+        <v xml:space="preserve">buried  </v>
+      </c>
+      <c r="D2">
+        <f>combined!AX2</f>
+        <v>4.49</v>
+      </c>
+      <c r="E2">
+        <f>combined!AD2</f>
+        <v>23.37</v>
+      </c>
+      <c r="F2">
+        <f>combined!AG2</f>
+        <v>4.47</v>
+      </c>
+      <c r="G2">
+        <f>E2*D2</f>
+        <v>104.93130000000001</v>
+      </c>
+      <c r="H2">
+        <f>combined!AI2</f>
+        <v>-0.85</v>
+      </c>
+      <c r="I2">
+        <f>(H2/(15.999*2))*-12.011</f>
+        <v>0.31906212888305513</v>
+      </c>
+      <c r="J2">
+        <f>(I2*1000)/(24*60*60)</f>
+        <v>3.6928487139242495E-3</v>
+      </c>
+      <c r="K2">
+        <f>G2/(J2*F2)</f>
+        <v>6356.7629158151303</v>
+      </c>
+      <c r="L2">
+        <f>1/K2*-1</f>
+        <v>-1.573127727498029E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>combined!B3</f>
+        <v>Amberly</v>
+      </c>
+      <c r="B3" t="str">
+        <f>combined!C3</f>
+        <v>Fall</v>
+      </c>
+      <c r="C3" t="str">
+        <f>combined!D3</f>
+        <v>daylight</v>
+      </c>
+      <c r="D3">
+        <f>combined!AX3</f>
+        <v>3.21</v>
+      </c>
+      <c r="E3">
+        <f>combined!AD3</f>
+        <v>28.94</v>
+      </c>
+      <c r="F3">
+        <f>combined!AG3</f>
+        <v>3.62</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G18" si="0">E3*D3</f>
+        <v>92.897400000000005</v>
+      </c>
+      <c r="H3">
+        <f>combined!AI3</f>
+        <v>-0.65</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I18" si="1">(H3/(15.999*2))*-12.011</f>
+        <v>0.24398868679292454</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J18" si="2">(I3*1000)/(24*60*60)</f>
+        <v>2.8239431341773673E-3</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K18" si="3">G3/(J3*F3)</f>
+        <v>9087.3873778785364</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L18" si="4">1/K3*-1</f>
+        <v>-1.1004262924174488E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>combined!B4</f>
+        <v>Amberly</v>
+      </c>
+      <c r="B4" t="str">
+        <f>combined!C4</f>
+        <v>Spring</v>
+      </c>
+      <c r="C4" t="str">
+        <f>combined!D4</f>
+        <v xml:space="preserve">buried  </v>
+      </c>
+      <c r="D4">
+        <f>combined!AX4</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E4">
+        <f>combined!AD4</f>
+        <v>27.33</v>
+      </c>
+      <c r="F4">
+        <f>combined!AG4</f>
+        <v>4.49</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>60.125999999999998</v>
+      </c>
+      <c r="H4">
+        <f>combined!AI4</f>
+        <v>-2.39</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0.897127632977061</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>1.0383421677975244E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>1289.6607428007708</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>-7.7539772035573377E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>combined!B5</f>
+        <v>Amberly</v>
+      </c>
+      <c r="B5" t="str">
+        <f>combined!C5</f>
+        <v>Spring</v>
+      </c>
+      <c r="C5" t="str">
+        <f>combined!D5</f>
+        <v>daylight</v>
+      </c>
+      <c r="D5">
+        <f>combined!AX5</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E5">
+        <f>combined!AD5</f>
+        <v>26.76</v>
+      </c>
+      <c r="F5">
+        <f>combined!AG5</f>
+        <v>3.91</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>61.548000000000002</v>
+      </c>
+      <c r="H5">
+        <f>combined!AI5</f>
+        <v>-3.41</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>1.2800021876367271</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>1.4814840134684341E-2</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>1062.5275958081495</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>-9.4115202649339993E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>combined!B6</f>
+        <v>Amberly</v>
+      </c>
+      <c r="B6" t="str">
+        <f>combined!C6</f>
+        <v>Summer</v>
+      </c>
+      <c r="C6" t="str">
+        <f>combined!D6</f>
+        <v xml:space="preserve">buried  </v>
+      </c>
+      <c r="D6">
+        <f>combined!AX6</f>
+        <v>3.36</v>
+      </c>
+      <c r="E6">
+        <f>combined!AD6</f>
+        <v>14.13</v>
+      </c>
+      <c r="F6">
+        <f>combined!AG6</f>
+        <v>3.73</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>47.476800000000004</v>
+      </c>
+      <c r="H6">
+        <f>combined!AI6</f>
+        <v>-3.63</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>1.3625829739358708</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>1.5770636272405911E-2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>807.09264936450541</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>-1.239015125199551E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>combined!B7</f>
+        <v>Amberly</v>
+      </c>
+      <c r="B7" t="str">
+        <f>combined!C7</f>
+        <v>Summer</v>
+      </c>
+      <c r="C7" t="str">
+        <f>combined!D7</f>
+        <v>daylight</v>
+      </c>
+      <c r="D7">
+        <f>combined!AX7</f>
+        <v>3.51</v>
+      </c>
+      <c r="E7">
+        <f>combined!AD7</f>
+        <v>2.82</v>
+      </c>
+      <c r="F7">
+        <f>combined!AG7</f>
+        <v>3.82</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>9.8981999999999992</v>
+      </c>
+      <c r="H7">
+        <f>combined!AI7</f>
+        <v>-1.5</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0.5630508156759797</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>6.5167918481016168E-3</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>397.61156913666838</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>-2.5150173627273825E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>combined!B8</f>
+        <v>Eastgate</v>
+      </c>
+      <c r="B8" t="str">
+        <f>combined!C8</f>
+        <v>Fall</v>
+      </c>
+      <c r="C8" t="str">
+        <f>combined!D8</f>
+        <v xml:space="preserve">buried  </v>
+      </c>
+      <c r="D8">
+        <f>combined!AX8</f>
+        <v>4.16</v>
+      </c>
+      <c r="E8">
+        <f>combined!AD8</f>
+        <v>2.14</v>
+      </c>
+      <c r="F8">
+        <f>combined!AG8</f>
+        <v>0.69</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>8.9024000000000001</v>
+      </c>
+      <c r="H8">
+        <f>combined!AI8</f>
+        <v>-0.1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>3.7536721045065315E-2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>4.3445278987344112E-4</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>29697.194462177795</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>-3.3673214527843536E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>combined!B9</f>
+        <v>Eastgate</v>
+      </c>
+      <c r="B9" t="str">
+        <f>combined!C9</f>
+        <v>Fall</v>
+      </c>
+      <c r="C9" t="str">
+        <f>combined!D9</f>
+        <v>daylight</v>
+      </c>
+      <c r="D9">
+        <f>combined!AX9</f>
+        <v>4.34</v>
+      </c>
+      <c r="E9">
+        <f>combined!AD9</f>
+        <v>3.22</v>
+      </c>
+      <c r="F9">
+        <f>combined!AG9</f>
+        <v>2.44</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>13.9748</v>
+      </c>
+      <c r="H9">
+        <f>combined!AI9</f>
+        <v>-7.08</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>2.6575998499906239</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>3.0759257523039631E-2</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>186.20010723244363</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>-5.3705661874385822E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>combined!B10</f>
+        <v>Eastgate</v>
+      </c>
+      <c r="B10" t="str">
+        <f>combined!C10</f>
+        <v>Spring</v>
+      </c>
+      <c r="C10" t="str">
+        <f>combined!D10</f>
+        <v xml:space="preserve">buried  </v>
+      </c>
+      <c r="D10">
+        <f>combined!AX10</f>
+        <v>3.61</v>
+      </c>
+      <c r="E10">
+        <f>combined!AD10</f>
+        <v>2.39</v>
+      </c>
+      <c r="F10">
+        <f>combined!AG10</f>
+        <v>0.6</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>8.6279000000000003</v>
+      </c>
+      <c r="H10" t="str">
+        <f>combined!AI10</f>
+        <v>NA</v>
+      </c>
+      <c r="I10" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J10" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K10" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L10" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>combined!B11</f>
+        <v>Eastgate</v>
+      </c>
+      <c r="B11" t="str">
+        <f>combined!C11</f>
+        <v>Spring</v>
+      </c>
+      <c r="C11" t="str">
+        <f>combined!D11</f>
+        <v>daylight</v>
+      </c>
+      <c r="D11">
+        <f>combined!AX11</f>
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f>combined!AD11</f>
+        <v>3.45</v>
+      </c>
+      <c r="F11">
+        <f>combined!AG11</f>
+        <v>2.29</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>13.8</v>
+      </c>
+      <c r="H11">
+        <f>combined!AI11</f>
+        <v>-3.86</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>1.4489174323395211</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>1.6769877689114827E-2</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>359.34673973645005</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>-2.7828275295705036E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>combined!B12</f>
+        <v>Eastgate</v>
+      </c>
+      <c r="B12" t="str">
+        <f>combined!C12</f>
+        <v>Summer</v>
+      </c>
+      <c r="C12" t="str">
+        <f>combined!D12</f>
+        <v xml:space="preserve">buried  </v>
+      </c>
+      <c r="D12">
+        <f>combined!AX12</f>
+        <v>4.2</v>
+      </c>
+      <c r="E12">
+        <f>combined!AD12</f>
+        <v>0.94</v>
+      </c>
+      <c r="F12">
+        <f>combined!AG12</f>
+        <v>0.63</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>3.948</v>
+      </c>
+      <c r="H12">
+        <f>combined!AI12</f>
+        <v>-0.23</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>8.6334458403650227E-2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>9.9924141670891466E-4</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="3"/>
+        <v>6271.4240641730585</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>-1.5945341755993321E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>combined!B13</f>
+        <v>Este</v>
+      </c>
+      <c r="B13" t="str">
+        <f>combined!C13</f>
+        <v>Fall</v>
+      </c>
+      <c r="C13" t="str">
+        <f>combined!D13</f>
+        <v xml:space="preserve">buried  </v>
+      </c>
+      <c r="D13">
+        <f>combined!AX13</f>
+        <v>2.8</v>
+      </c>
+      <c r="E13">
+        <f>combined!AD13</f>
+        <v>6.13</v>
+      </c>
+      <c r="F13">
+        <f>combined!AG13</f>
+        <v>0.9</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>17.163999999999998</v>
+      </c>
+      <c r="H13">
+        <f>combined!AI13</f>
+        <v>-2.8039999999999998</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>1.0525296581036314</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>1.218205622805129E-2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="3"/>
+        <v>1565.508380038222</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>-6.3877013547227704E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>combined!B14</f>
+        <v>Este</v>
+      </c>
+      <c r="B14" t="str">
+        <f>combined!C14</f>
+        <v>Fall</v>
+      </c>
+      <c r="C14" t="str">
+        <f>combined!D14</f>
+        <v>daylight</v>
+      </c>
+      <c r="D14">
+        <f>combined!AX14</f>
+        <v>3.26</v>
+      </c>
+      <c r="E14">
+        <f>combined!AD14</f>
+        <v>5.15</v>
+      </c>
+      <c r="F14">
+        <f>combined!AG14</f>
+        <v>1.95</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>16.789000000000001</v>
+      </c>
+      <c r="H14">
+        <f>combined!AI14</f>
+        <v>-2.88</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>1.081057566097881</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>1.2512240348355103E-2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>688.10567492618975</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="4"/>
+        <v>-1.4532651545233453E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>combined!B15</f>
+        <v>Este</v>
+      </c>
+      <c r="B15" t="str">
+        <f>combined!C15</f>
+        <v>Spring</v>
+      </c>
+      <c r="C15" t="str">
+        <f>combined!D15</f>
+        <v xml:space="preserve">buried  </v>
+      </c>
+      <c r="D15">
+        <f>combined!AX15</f>
+        <v>2.77</v>
+      </c>
+      <c r="E15">
+        <f>combined!AD15</f>
+        <v>12.26</v>
+      </c>
+      <c r="F15">
+        <f>combined!AG15</f>
+        <v>1.06</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>33.9602</v>
+      </c>
+      <c r="H15">
+        <f>combined!AI15</f>
+        <v>-0.51200000000000001</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0.19218801175073441</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>2.2243982841520186E-3</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>14402.962255707427</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="4"/>
+        <v>-6.9430161812979293E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>combined!B16</f>
+        <v>Este</v>
+      </c>
+      <c r="B16" t="str">
+        <f>combined!C16</f>
+        <v>Spring</v>
+      </c>
+      <c r="C16" t="str">
+        <f>combined!D16</f>
+        <v>daylight</v>
+      </c>
+      <c r="D16">
+        <f>combined!AX16</f>
+        <v>2.94</v>
+      </c>
+      <c r="E16">
+        <f>combined!AD16</f>
+        <v>11.72</v>
+      </c>
+      <c r="F16">
+        <f>combined!AG16</f>
+        <v>2.23</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>34.456800000000001</v>
+      </c>
+      <c r="H16">
+        <f>combined!AI16</f>
+        <v>-5.53</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>2.0757806737921118</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>2.4025239280001293E-2</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>643.13531451441895</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="4"/>
+        <v>-1.5548827399643286E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>combined!B17</f>
+        <v>Este</v>
+      </c>
+      <c r="B17" t="str">
+        <f>combined!C17</f>
+        <v>Summer</v>
+      </c>
+      <c r="C17" t="str">
+        <f>combined!D17</f>
+        <v xml:space="preserve">buried  </v>
+      </c>
+      <c r="D17">
+        <f>combined!AX17</f>
+        <v>2.42</v>
+      </c>
+      <c r="E17">
+        <f>combined!AD17</f>
+        <v>8.9</v>
+      </c>
+      <c r="F17">
+        <f>combined!AG17</f>
+        <v>0.89</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>21.538</v>
+      </c>
+      <c r="H17">
+        <f>combined!AI17</f>
+        <v>-4.8319999999999999</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>1.8137743608975558</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>2.0992758806684674E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>1152.7784519819306</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="4"/>
+        <v>-8.6746937217705268E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>combined!B18</f>
+        <v>Este</v>
+      </c>
+      <c r="B18" t="str">
+        <f>combined!C18</f>
+        <v>Summer</v>
+      </c>
+      <c r="C18" t="str">
+        <f>combined!D18</f>
+        <v>daylight</v>
+      </c>
+      <c r="D18">
+        <f>combined!AX18</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E18">
+        <f>combined!AD18</f>
+        <v>3.82</v>
+      </c>
+      <c r="F18">
+        <f>combined!AG18</f>
+        <v>1.92</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>8.4039999999999999</v>
+      </c>
+      <c r="H18">
+        <f>combined!AI18</f>
+        <v>-8.35</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>3.1343162072629531</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>3.6276807954432326E-2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>120.65789632956222</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="4"/>
+        <v>-8.2878952013933915E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>